<commit_message>
Update Estimates and Actuals.xlsx
</commit_message>
<xml_diff>
--- a/Estimates and Actuals.xlsx
+++ b/Estimates and Actuals.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnq\Documents\GitHub\SMP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{091E9654-DB50-4DF6-B21F-5094E7C794CD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DA6C266-35D1-4D98-BA55-D9A8B385C8A5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5568" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="67">
   <si>
     <t>Documentation</t>
   </si>
@@ -311,6 +311,9 @@
   </si>
   <si>
     <t>Research</t>
+  </si>
+  <si>
+    <t>Loc Implementation/refinement</t>
   </si>
 </sst>
 </file>
@@ -846,7 +849,7 @@
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -891,11 +894,11 @@
       </c>
       <c r="F2" s="5">
         <f>SUM(F3:F5)</f>
-        <v>12</v>
+        <v>18.75</v>
       </c>
       <c r="G2" s="5">
         <f>(E2-F2)</f>
-        <v>-12</v>
+        <v>-18.75</v>
       </c>
       <c r="H2" s="5">
         <f>E2/F2*100</f>
@@ -910,12 +913,11 @@
         <v>108</v>
       </c>
       <c r="F3" s="4">
-        <f>SUM(Weekly!C6:N6)</f>
-        <v>3</v>
+        <v>3.75</v>
       </c>
       <c r="G3" s="10">
         <f t="shared" ref="G3:G7" si="0">(E3-F3)</f>
-        <v>-3</v>
+        <v>-3.75</v>
       </c>
       <c r="H3" s="10">
         <f t="shared" ref="H3:H7" si="1">E3/F3*100</f>
@@ -950,12 +952,11 @@
         <v>144</v>
       </c>
       <c r="F5" s="4">
-        <f>SUM(Weekly!C8:N8)</f>
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="G5" s="10">
         <f t="shared" si="0"/>
-        <v>-8</v>
+        <v>-14</v>
       </c>
       <c r="H5" s="10">
         <f t="shared" si="1"/>
@@ -980,15 +981,15 @@
       </c>
       <c r="F7" s="5">
         <f>SUM(F13:F15)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G7" s="5">
         <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+      <c r="H7" s="5">
+        <f t="shared" si="1"/>
         <v>0</v>
-      </c>
-      <c r="H7" s="5" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -1013,7 +1014,9 @@
         <v>36</v>
       </c>
       <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
+      <c r="F9" s="5">
+        <v>2</v>
+      </c>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
     </row>
@@ -1071,6 +1074,9 @@
       <c r="C14" s="4">
         <v>24</v>
       </c>
+      <c r="F14" s="4">
+        <v>4</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
@@ -1096,7 +1102,7 @@
         <v>12</v>
       </c>
       <c r="F17" s="4">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
@@ -1265,10 +1271,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1345,6 +1351,9 @@
       <c r="E6" s="7">
         <v>2</v>
       </c>
+      <c r="F6" s="7">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
@@ -1364,6 +1373,9 @@
       <c r="E8" s="7">
         <v>8</v>
       </c>
+      <c r="F8" s="7">
+        <v>6</v>
+      </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -1376,6 +1388,17 @@
       </c>
       <c r="E10" s="7">
         <v>12</v>
+      </c>
+      <c r="F10" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>66</v>
+      </c>
+      <c r="F11" s="7">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created Client minutes, weekly status report updated actuals
</commit_message>
<xml_diff>
--- a/Estimates and Actuals.xlsx
+++ b/Estimates and Actuals.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnq\Documents\GitHub\SMP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C5DFE62-EB84-41B5-840A-7D6FF3B93ED3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{217D2F40-72DE-49F1-A9D6-3DE0FB353AA7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1680" yWindow="816" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1680" yWindow="816" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="3" r:id="rId1"/>
@@ -845,7 +845,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -891,11 +891,11 @@
       </c>
       <c r="F2" s="5">
         <f>SUM(F3:F5)</f>
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="G2" s="5">
         <f>(E2-F2)</f>
-        <v>-38</v>
+        <v>-58</v>
       </c>
       <c r="H2" s="5">
         <f>E2/F2*100</f>
@@ -910,11 +910,11 @@
         <v>108</v>
       </c>
       <c r="F3" s="4">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G3" s="4">
         <f t="shared" ref="G3:G7" si="0">(E3-F3)</f>
-        <v>-14</v>
+        <v>-18</v>
       </c>
       <c r="H3" s="4">
         <f t="shared" ref="H3:H7" si="1">E3/F3*100</f>
@@ -949,11 +949,11 @@
         <v>144</v>
       </c>
       <c r="F5" s="4">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="G5" s="4">
         <f t="shared" si="0"/>
-        <v>-23</v>
+        <v>-39</v>
       </c>
       <c r="H5" s="4">
         <f t="shared" si="1"/>
@@ -977,11 +977,11 @@
       </c>
       <c r="F7" s="5">
         <f>SUM(F13:F15)</f>
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G7" s="5">
         <f t="shared" si="0"/>
-        <v>-17</v>
+        <v>-19</v>
       </c>
       <c r="H7" s="5">
         <f t="shared" si="1"/>
@@ -1011,7 +1011,7 @@
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="5">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
@@ -1053,7 +1053,9 @@
         <v>12</v>
       </c>
       <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
+      <c r="F12" s="5">
+        <v>8</v>
+      </c>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
     </row>
@@ -1084,7 +1086,7 @@
         <v>32</v>
       </c>
       <c r="F15" s="4">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
@@ -1278,8 +1280,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1368,6 +1370,9 @@
       <c r="J6" s="7">
         <v>2</v>
       </c>
+      <c r="K6" s="7">
+        <v>2</v>
+      </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
@@ -1399,6 +1404,9 @@
       <c r="J8" s="7">
         <v>3</v>
       </c>
+      <c r="K8" s="7">
+        <v>3</v>
+      </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -1426,6 +1434,9 @@
       <c r="J11" s="7">
         <v>1</v>
       </c>
+      <c r="K11" s="7">
+        <v>3</v>
+      </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
@@ -1453,6 +1464,9 @@
       <c r="J14" s="7">
         <v>3</v>
       </c>
+      <c r="K14" s="7">
+        <v>3</v>
+      </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
@@ -1461,6 +1475,9 @@
       <c r="J15" s="7">
         <v>2</v>
       </c>
+      <c r="K15" s="7">
+        <v>8</v>
+      </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
@@ -1468,6 +1485,9 @@
       </c>
       <c r="J16" s="7">
         <v>5</v>
+      </c>
+      <c r="K16" s="7">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
files for last week
</commit_message>
<xml_diff>
--- a/Estimates and Actuals.xlsx
+++ b/Estimates and Actuals.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnq\Documents\GitHub\SMP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{217D2F40-72DE-49F1-A9D6-3DE0FB353AA7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8180EB5-2B01-4338-BC3B-FECE79997947}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1680" yWindow="816" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1680" yWindow="816" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="3" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="75">
   <si>
     <t>Documentation</t>
   </si>
@@ -329,6 +329,15 @@
   </si>
   <si>
     <t>PHP script DB</t>
+  </si>
+  <si>
+    <t>DB Logic/Android Logic</t>
+  </si>
+  <si>
+    <t>DB Translator Logic</t>
+  </si>
+  <si>
+    <t>Android/DB logic</t>
   </si>
 </sst>
 </file>
@@ -843,10 +852,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -972,7 +981,7 @@
         <v>230</v>
       </c>
       <c r="E7" s="5">
-        <f>SUM(E13:E18)</f>
+        <f>SUM(E13:E19)</f>
         <v>0</v>
       </c>
       <c r="F7" s="5">
@@ -1011,7 +1020,7 @@
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="5">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
@@ -1054,7 +1063,7 @@
       </c>
       <c r="E12" s="5"/>
       <c r="F12" s="5">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
@@ -1113,63 +1122,58 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
+        <v>74</v>
+      </c>
+      <c r="F18" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
         <v>49</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C19" s="4">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
+    <row r="20" spans="1:8" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>63</v>
       </c>
-      <c r="C20" s="6">
+      <c r="C21" s="6">
         <v>182</v>
       </c>
-      <c r="E20" s="5">
-        <f>SUM(E24:E26)</f>
+      <c r="E21" s="5">
+        <f>SUM(E25:E27)</f>
         <v>0</v>
       </c>
-      <c r="F20" s="5">
-        <f>SUM(F24:F26)</f>
+      <c r="F21" s="5">
+        <f>SUM(F25:F27)</f>
         <v>2</v>
       </c>
-      <c r="G20" s="5">
-        <f>(E20-F20)</f>
+      <c r="G21" s="5">
+        <f>(E21-F21)</f>
         <v>-2</v>
       </c>
-      <c r="H20" s="5">
-        <f>E20/F20*100</f>
+      <c r="H21" s="5">
+        <f>E21/F21*100</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="1"/>
-      <c r="B21" t="s">
-        <v>57</v>
-      </c>
-      <c r="C21" s="9">
-        <v>2</v>
-      </c>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C22" s="9">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
@@ -1179,10 +1183,10 @@
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C23" s="9">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
@@ -1192,81 +1196,94 @@
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" t="s">
-        <v>51</v>
-      </c>
-      <c r="C24" s="4">
-        <v>12</v>
-      </c>
-      <c r="F24" s="4">
-        <v>2</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="C24" s="9">
+        <v>24</v>
+      </c>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" s="4">
+        <v>12</v>
+      </c>
+      <c r="F25" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="1"/>
+      <c r="B26" t="s">
         <v>53</v>
       </c>
-      <c r="C25" s="4">
+      <c r="C26" s="4">
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B26" t="s">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
         <v>60</v>
       </c>
-      <c r="C26" s="4">
+      <c r="C27" s="4">
         <v>92</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G27" s="5"/>
-      <c r="H27" s="5"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
+    <row r="28" spans="1:8" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C28" s="6">
+      <c r="C29" s="6">
         <v>124</v>
       </c>
-      <c r="E28" s="5">
-        <f>SUM(E29:E31)</f>
+      <c r="E29" s="5">
+        <f>SUM(E30:E32)</f>
         <v>0</v>
       </c>
-      <c r="F28" s="5">
-        <f>SUM(F29:F31)</f>
+      <c r="F29" s="5">
+        <f>SUM(F30:F32)</f>
         <v>0</v>
       </c>
-      <c r="G28" s="5">
-        <f>(E28-F28)</f>
+      <c r="G29" s="5">
+        <f>(E29-F29)</f>
         <v>0</v>
       </c>
-      <c r="H28" s="5" t="e">
-        <f>E28/F28*100</f>
+      <c r="H29" s="5" t="e">
+        <f>E29/F29*100</f>
         <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B29" t="s">
-        <v>47</v>
-      </c>
-      <c r="C29" s="4">
-        <v>16</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>50</v>
-      </c>
-      <c r="C30" s="9">
-        <v>8</v>
+        <v>47</v>
+      </c>
+      <c r="C30" s="4">
+        <v>16</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
+        <v>50</v>
+      </c>
+      <c r="C31" s="9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
         <v>61</v>
       </c>
-      <c r="C31" s="4">
+      <c r="C32" s="4">
         <v>100</v>
       </c>
     </row>
@@ -1278,10 +1295,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:N16"/>
+  <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1453,6 +1470,9 @@
       <c r="G13" s="7">
         <v>4</v>
       </c>
+      <c r="M13" s="7">
+        <v>4</v>
+      </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
@@ -1478,6 +1498,9 @@
       <c r="K15" s="7">
         <v>8</v>
       </c>
+      <c r="M15" s="7">
+        <v>8</v>
+      </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
@@ -1488,6 +1511,25 @@
       </c>
       <c r="K16" s="7">
         <v>2</v>
+      </c>
+      <c r="M16" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>72</v>
+      </c>
+      <c r="M17" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>73</v>
+      </c>
+      <c r="M18" s="7">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Some changes plus docs
</commit_message>
<xml_diff>
--- a/Estimates and Actuals.xlsx
+++ b/Estimates and Actuals.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnq\Documents\GitHub\SMP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0649C290-A72B-45A1-AEE5-0EC69AB46552}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4197B3ED-EE0E-4ED8-97F4-62A5341DF773}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1680" yWindow="816" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="3" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="76">
   <si>
     <t>Documentation</t>
   </si>
@@ -338,6 +338,9 @@
   </si>
   <si>
     <t>Android/DB logic</t>
+  </si>
+  <si>
+    <t>PHASE2: W1</t>
   </si>
 </sst>
 </file>
@@ -854,8 +857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -900,11 +903,11 @@
       </c>
       <c r="F2" s="5">
         <f>SUM(F3:F5)</f>
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="G2" s="5">
         <f>(E2-F2)</f>
-        <v>-58</v>
+        <v>-70</v>
       </c>
       <c r="H2" s="5">
         <f>E2/F2*100</f>
@@ -958,11 +961,11 @@
         <v>144</v>
       </c>
       <c r="F5" s="4">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="G5" s="4">
         <f t="shared" si="0"/>
-        <v>-39</v>
+        <v>-51</v>
       </c>
       <c r="H5" s="4">
         <f t="shared" si="1"/>
@@ -1117,7 +1120,7 @@
         <v>12</v>
       </c>
       <c r="F17" s="4">
-        <v>16</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
@@ -1295,10 +1298,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:N18"/>
+  <dimension ref="A1:S18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1306,19 +1309,20 @@
     <col min="1" max="1" width="5.44140625" customWidth="1"/>
     <col min="2" max="2" width="21.44140625" customWidth="1"/>
     <col min="3" max="14" width="5.6640625" style="7" customWidth="1"/>
+    <col min="15" max="15" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C4" s="8" t="s">
         <v>15</v>
       </c>
@@ -1355,14 +1359,29 @@
       <c r="N4" s="8" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O4" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="8"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -1391,7 +1410,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>14</v>
       </c>
@@ -1401,8 +1420,11 @@
       <c r="E7" s="7">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>0</v>
       </c>
@@ -1425,12 +1447,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>65</v>
       </c>
@@ -1441,7 +1466,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>66</v>
       </c>
@@ -1455,7 +1480,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>67</v>
       </c>
@@ -1463,7 +1488,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>68</v>
       </c>
@@ -1474,7 +1499,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>69</v>
       </c>
@@ -1488,7 +1513,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>70</v>
       </c>
@@ -1505,7 +1530,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>71</v>
       </c>

</xml_diff>

<commit_message>
oliver bug fixes johns help
</commit_message>
<xml_diff>
--- a/Estimates and Actuals.xlsx
+++ b/Estimates and Actuals.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnq\Documents\GitHub\SMP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CE5505F-C656-40F2-8E75-E9B7408E2388}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3341BCE6-5627-4F5E-B6C8-2F440292F57D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="3" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="92">
   <si>
     <t>Documentation</t>
   </si>
@@ -365,6 +365,30 @@
   </si>
   <si>
     <t>Promotions</t>
+  </si>
+  <si>
+    <t>KPI reports</t>
+  </si>
+  <si>
+    <t>KPI report emailer</t>
+  </si>
+  <si>
+    <t>Miscellaneous bug fixes</t>
+  </si>
+  <si>
+    <t>Saved state</t>
+  </si>
+  <si>
+    <t>Business testing</t>
+  </si>
+  <si>
+    <t>Settings</t>
+  </si>
+  <si>
+    <t>Admin admin</t>
+  </si>
+  <si>
+    <t>Misellanous bug fixing</t>
   </si>
 </sst>
 </file>
@@ -879,10 +903,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1030,7 +1054,7 @@
         <v>59</v>
       </c>
       <c r="C8" s="4">
-        <v>80</v>
+        <v>215</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
@@ -1178,11 +1202,11 @@
         <v>182</v>
       </c>
       <c r="E21" s="5">
-        <f>SUM(E25:E27)</f>
+        <f>SUM(E25:E28)</f>
         <v>0</v>
       </c>
       <c r="F21" s="5">
-        <f>SUM(F25:F27)</f>
+        <f>SUM(F25:F28)</f>
         <v>2</v>
       </c>
       <c r="G21" s="5">
@@ -1255,62 +1279,71 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" s="1"/>
       <c r="B27" t="s">
+        <v>91</v>
+      </c>
+      <c r="C27" s="4">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
         <v>60</v>
       </c>
-      <c r="C27" s="4">
+      <c r="C28" s="4">
         <v>92</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G28" s="5"/>
-      <c r="H28" s="5"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
+    <row r="29" spans="1:8" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C29" s="6">
+      <c r="C30" s="6">
         <v>124</v>
       </c>
-      <c r="E29" s="5">
-        <f>SUM(E30:E32)</f>
+      <c r="E30" s="5">
+        <f>SUM(E31:E33)</f>
         <v>0</v>
       </c>
-      <c r="F29" s="5">
-        <f>SUM(F30:F32)</f>
+      <c r="F30" s="5">
+        <f>SUM(F31:F33)</f>
         <v>0</v>
       </c>
-      <c r="G29" s="5">
-        <f>(E29-F29)</f>
+      <c r="G30" s="5">
+        <f>(E30-F30)</f>
         <v>0</v>
       </c>
-      <c r="H29" s="5" t="e">
-        <f>E29/F29*100</f>
+      <c r="H30" s="5" t="e">
+        <f>E30/F30*100</f>
         <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B30" t="s">
-        <v>47</v>
-      </c>
-      <c r="C30" s="4">
-        <v>16</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
-        <v>50</v>
-      </c>
-      <c r="C31" s="9">
-        <v>8</v>
+        <v>47</v>
+      </c>
+      <c r="C31" s="4">
+        <v>16</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
+        <v>50</v>
+      </c>
+      <c r="C32" s="9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
         <v>61</v>
       </c>
-      <c r="C32" s="4">
+      <c r="C33" s="4">
         <v>100</v>
       </c>
     </row>
@@ -1322,10 +1355,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:S26"/>
+  <dimension ref="A1:S38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P23" sqref="P23"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1473,6 +1506,9 @@
       <c r="P8">
         <v>3.5</v>
       </c>
+      <c r="Q8">
+        <v>7</v>
+      </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -1577,7 +1613,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>72</v>
       </c>
@@ -1588,15 +1624,18 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>73</v>
       </c>
       <c r="M18" s="7">
         <v>8</v>
       </c>
-    </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="Q18">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>76</v>
       </c>
@@ -1604,15 +1643,18 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>77</v>
       </c>
       <c r="P20">
         <v>17</v>
       </c>
-    </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="Q20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>78</v>
       </c>
@@ -1620,7 +1662,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>79</v>
       </c>
@@ -1628,7 +1670,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>80</v>
       </c>
@@ -1636,7 +1678,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>81</v>
       </c>
@@ -1644,7 +1686,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>82</v>
       </c>
@@ -1652,12 +1694,81 @@
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>83</v>
       </c>
       <c r="P26">
         <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q27">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q28">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q29">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q30">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q31">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q32">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q36">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q37">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>